<commit_message>
fix render text thumb issue
</commit_message>
<xml_diff>
--- a/tests/videos/horizon/videos-meta.xlsx
+++ b/tests/videos/horizon/videos-meta.xlsx
@@ -616,9 +616,19 @@
           <t>OP</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>op-test</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>who is there</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>4444</v>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>OP</t>
@@ -635,12 +645,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2023-10-12T00:00:00+00:00</t>
+          <t>2023-10-13T00:00:00+00:00</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>7:45</t>
+          <t>19:45</t>
         </is>
       </c>
       <c r="N2" t="b">

</xml_diff>

<commit_message>
fix issue about thumblocalfile
</commit_message>
<xml_diff>
--- a/tests/videos/horizon/videos-meta.xlsx
+++ b/tests/videos/horizon/videos-meta.xlsx
@@ -618,39 +618,35 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>op-test</t>
+          <t>中文</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>who is there</t>
+          <t>英文</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>4444</v>
+        <v>123</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>OP</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>/Users/wenke/github/tiktoka-studio-uploader-app/tests/videos/horizon/1920x1080/bg2.jpg</t>
+        </is>
+      </c>
       <c r="J2" t="n">
         <v>2</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2023-10-13T00:00:00+00:00</t>
-        </is>
-      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>19:45</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="N2" t="b">

</xml_diff>

<commit_message>
if set combox variable trace,it will run twice and overwrite. fix thumbview videometa sync if you change videometa files
</commit_message>
<xml_diff>
--- a/tests/videos/horizon/videos-meta.xlsx
+++ b/tests/videos/horizon/videos-meta.xlsx
@@ -642,7 +642,11 @@
       <c r="J2" t="n">
         <v>2</v>
       </c>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>['/Users/wenke/github/tiktoka-studio-uploader-app/tests/videos/horizon/OP.png']</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>

</xml_diff>